<commit_message>
default : continue to practice
</commit_message>
<xml_diff>
--- a/LCProblems.xlsx
+++ b/LCProblems.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="6225" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6228" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Union Find" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="216">
   <si>
     <t>https://leetcode.com/problems/regions-cut-by-slashes</t>
   </si>
@@ -604,18 +604,9 @@
     <t>2189. Number of Ways to Build House of Cards</t>
   </si>
   <si>
-    <t>https://leetcode.com/problems/fair-distribution-of-cookies/</t>
-  </si>
-  <si>
     <t>dfs generic dp</t>
   </si>
   <si>
-    <t>similar to find minimum time to finish all jobs, when n is smaller than 32, we can use bit masking to find subsets</t>
-  </si>
-  <si>
-    <t>2305. Fair Distribution of Cookie</t>
-  </si>
-  <si>
     <t>https://leetcode.com/problems/maximum-subarray/</t>
   </si>
   <si>
@@ -668,6 +659,48 @@
   </si>
   <si>
     <t>kadane with dp</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/shortest-way-to-form-string/</t>
+  </si>
+  <si>
+    <t>Greedy</t>
+  </si>
+  <si>
+    <t>1055. Shortest Way to Form String</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/last-stone-weight-ii/</t>
+  </si>
+  <si>
+    <t>1049. Last Stone Weight II</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/design-an-expression-tree-with-evaluate-function/</t>
+  </si>
+  <si>
+    <t>1628. Design an Expression Tree With Evaluate Function</t>
+  </si>
+  <si>
+    <t>Stack</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-subarray-min-product/</t>
+  </si>
+  <si>
+    <t>1856. Maximum Subarray Min-Product</t>
+  </si>
+  <si>
+    <t>Monotonic stack</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-window-substring/</t>
+  </si>
+  <si>
+    <t>76. Minimum Window Substring</t>
+  </si>
+  <si>
+    <t>sliding window</t>
   </si>
 </sst>
 </file>
@@ -1060,8 +1093,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table143" displayName="Table143" ref="A1:D14" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="A1:D14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table143" displayName="Table143" ref="A1:D18" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="A1:D18"/>
   <tableColumns count="4">
     <tableColumn id="4" name="Date" dataDxfId="21"/>
     <tableColumn id="1" name="Name" dataDxfId="20"/>
@@ -1380,16 +1413,16 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="46.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="4"/>
+    <col min="1" max="1" width="12.109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="31.109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="46.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>6</v>
       </c>
@@ -1403,7 +1436,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>44640</v>
       </c>
@@ -1417,7 +1450,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>44642</v>
       </c>
@@ -1431,7 +1464,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>44649</v>
       </c>
@@ -1445,7 +1478,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>44671</v>
       </c>
@@ -1459,7 +1492,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>44672</v>
       </c>
@@ -1473,7 +1506,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>44674</v>
       </c>
@@ -1502,20 +1535,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView topLeftCell="A26" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="50.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="50.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="60.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50" style="1" customWidth="1"/>
-    <col min="4" max="4" width="75.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="50.140625" style="1"/>
+    <col min="4" max="4" width="75.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="50.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>6</v>
       </c>
@@ -1529,7 +1562,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>44641</v>
       </c>
@@ -1543,7 +1576,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>44641</v>
       </c>
@@ -1557,7 +1590,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>44642</v>
       </c>
@@ -1571,7 +1604,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>44643</v>
       </c>
@@ -1585,7 +1618,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>44646</v>
       </c>
@@ -1599,7 +1632,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>44659</v>
       </c>
@@ -1613,7 +1646,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>44659</v>
       </c>
@@ -1627,7 +1660,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>44660</v>
       </c>
@@ -1639,7 +1672,7 @@
       </c>
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>44662</v>
       </c>
@@ -1653,7 +1686,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>44664</v>
       </c>
@@ -1667,7 +1700,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>44664</v>
       </c>
@@ -1681,7 +1714,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>44665</v>
       </c>
@@ -1693,7 +1726,7 @@
       </c>
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>44669</v>
       </c>
@@ -1707,7 +1740,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>44677</v>
       </c>
@@ -1721,7 +1754,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>44680</v>
       </c>
@@ -1735,7 +1768,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>44683</v>
       </c>
@@ -1749,7 +1782,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>44692</v>
       </c>
@@ -1763,7 +1796,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>44692</v>
       </c>
@@ -1777,7 +1810,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>44693</v>
       </c>
@@ -1791,7 +1824,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>44693</v>
       </c>
@@ -1805,7 +1838,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>44693</v>
       </c>
@@ -1819,7 +1852,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>44695</v>
       </c>
@@ -1833,7 +1866,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>44696</v>
       </c>
@@ -1847,7 +1880,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>44697</v>
       </c>
@@ -1861,10 +1894,10 @@
         <v>147</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <f ca="1">TODAY()</f>
-        <v>44748</v>
+        <v>44770</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>155</v>
@@ -1876,10 +1909,10 @@
         <v>156</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <f ca="1">TODAY()</f>
-        <v>44748</v>
+        <v>44770</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>158</v>
@@ -1891,7 +1924,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>44707</v>
       </c>
@@ -1903,7 +1936,7 @@
       </c>
       <c r="D28" s="4"/>
     </row>
-    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>44710</v>
       </c>
@@ -1915,7 +1948,7 @@
       </c>
       <c r="D29" s="4"/>
     </row>
-    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>44713</v>
       </c>
@@ -1929,7 +1962,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>44714</v>
       </c>
@@ -1943,7 +1976,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>44717</v>
       </c>
@@ -1957,7 +1990,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>44719</v>
       </c>
@@ -1971,7 +2004,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>44725</v>
       </c>
@@ -1985,7 +2018,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>44726</v>
       </c>
@@ -1994,92 +2027,92 @@
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="3">
+        <v>44739</v>
+      </c>
+      <c r="B36" t="s">
+        <v>185</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="3">
-        <v>44734</v>
-      </c>
-      <c r="B36" s="4" t="s">
+      <c r="D36" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C36" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
-        <v>44739</v>
+        <v>44740</v>
       </c>
       <c r="B37" t="s">
-        <v>188</v>
+        <v>82</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>187</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>44740</v>
       </c>
       <c r="B38" t="s">
-        <v>82</v>
+        <v>190</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
-        <v>44740</v>
+        <v>44745</v>
       </c>
       <c r="B39" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
-        <v>44745</v>
+        <f ca="1">TODAY()</f>
+        <v>44770</v>
       </c>
       <c r="B40" t="s">
+        <v>200</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="C40" s="5" t="s">
-        <v>198</v>
-      </c>
       <c r="D40" s="4" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
-        <f ca="1">TODAY()</f>
-        <v>44748</v>
-      </c>
-      <c r="B41" t="s">
-        <v>203</v>
+        <v>44751</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>206</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>204</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -2092,7 +2125,7 @@
     <hyperlink ref="C17" r:id="rId6"/>
     <hyperlink ref="C19" r:id="rId7"/>
     <hyperlink ref="C28" r:id="rId8"/>
-    <hyperlink ref="C41" r:id="rId9"/>
+    <hyperlink ref="C40" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId10"/>
@@ -2113,16 +2146,16 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.42578125" customWidth="1"/>
-    <col min="4" max="4" width="54.85546875" customWidth="1"/>
-    <col min="11" max="11" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.44140625" customWidth="1"/>
+    <col min="4" max="4" width="54.88671875" customWidth="1"/>
+    <col min="11" max="11" width="45.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
@@ -2136,7 +2169,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="12">
         <v>44650</v>
       </c>
@@ -2150,19 +2183,19 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="13"/>
       <c r="B3" s="10"/>
       <c r="C3" s="9"/>
       <c r="D3" s="8"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="15"/>
       <c r="B4" s="16"/>
       <c r="C4" s="17"/>
       <c r="D4" s="16"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K9" s="6"/>
     </row>
   </sheetData>
@@ -2178,22 +2211,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="4"/>
+    <col min="1" max="1" width="9.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>6</v>
       </c>
@@ -2207,7 +2240,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>44643</v>
       </c>
@@ -2221,7 +2254,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>44649</v>
       </c>
@@ -2235,7 +2268,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>44665</v>
       </c>
@@ -2249,7 +2282,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>44670</v>
       </c>
@@ -2263,7 +2296,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>44670</v>
       </c>
@@ -2277,7 +2310,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>44672</v>
       </c>
@@ -2291,7 +2324,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>44672</v>
       </c>
@@ -2305,7 +2338,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>44673</v>
       </c>
@@ -2319,7 +2352,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>44698</v>
       </c>
@@ -2333,7 +2366,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>44713</v>
       </c>
@@ -2347,7 +2380,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>44724</v>
       </c>
@@ -2361,38 +2394,97 @@
         <v>177</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>44741</v>
       </c>
       <c r="B13" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>44744</v>
       </c>
       <c r="B14" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>201</v>
+        <v>198</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>44750</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>44759</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>44761</v>
+      </c>
+      <c r="B17" t="s">
+        <v>211</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>44770</v>
+      </c>
+      <c r="B18" t="s">
+        <v>214</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>215</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C16" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2405,16 +2497,16 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="49.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" customWidth="1"/>
+    <col min="2" max="2" width="49.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55" customWidth="1"/>
-    <col min="4" max="4" width="44.7109375" customWidth="1"/>
-    <col min="14" max="14" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.6640625" customWidth="1"/>
+    <col min="14" max="14" width="44.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -2428,7 +2520,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>44649</v>
       </c>
@@ -2442,7 +2534,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>44650</v>
       </c>
@@ -2456,7 +2548,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>44651</v>
       </c>
@@ -2470,7 +2562,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>44651</v>
       </c>
@@ -2484,7 +2576,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>44666</v>
       </c>
@@ -2517,18 +2609,18 @@
       <selection sqref="A1:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="65.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="10" width="8.85546875" style="1"/>
-    <col min="11" max="11" width="42.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="10" width="8.88671875" style="1"/>
+    <col min="11" max="11" width="42.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>6</v>
       </c>
@@ -2542,7 +2634,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>44648</v>
       </c>
@@ -2556,7 +2648,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>44649</v>
       </c>
@@ -2570,7 +2662,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>44652</v>
       </c>
@@ -2584,7 +2676,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>44654</v>
       </c>
@@ -2598,7 +2690,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>44678</v>
       </c>
@@ -2627,20 +2719,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.28515625" style="1"/>
+    <col min="1" max="1" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -2654,7 +2746,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>44699</v>
       </c>
@@ -2668,22 +2760,22 @@
         <v>153</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="C3" s="5"/>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="C4" s="5"/>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="C5" s="5"/>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="C6" s="5"/>
       <c r="D6" s="4"/>

</xml_diff>

<commit_message>
Medication Planning Service... Basically a todo list but involves capacity planning and tracking
</commit_message>
<xml_diff>
--- a/LCProblems.xlsx
+++ b/LCProblems.xlsx
@@ -9,16 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6228" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6228" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Union Find" sheetId="1" r:id="rId1"/>
-    <sheet name="Dynamic Programming" sheetId="2" r:id="rId2"/>
-    <sheet name="KMP Pattern-Matching" sheetId="8" r:id="rId3"/>
-    <sheet name="Data Structure Question" sheetId="3" r:id="rId4"/>
-    <sheet name="BackTracking" sheetId="5" r:id="rId5"/>
-    <sheet name="DFS BFS Graph Tree" sheetId="4" r:id="rId6"/>
-    <sheet name="Merge Sort" sheetId="9" r:id="rId7"/>
+    <sheet name="Greedy" sheetId="11" r:id="rId2"/>
+    <sheet name="Dynamic Programming" sheetId="2" r:id="rId3"/>
+    <sheet name="KMP Pattern-Matching" sheetId="8" r:id="rId4"/>
+    <sheet name="DSA" sheetId="3" r:id="rId5"/>
+    <sheet name="BackTracking" sheetId="5" r:id="rId6"/>
+    <sheet name="DFS BFS Graph Tree" sheetId="4" r:id="rId7"/>
+    <sheet name="Merge Sort" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="283">
   <si>
     <t>https://leetcode.com/problems/regions-cut-by-slashes</t>
   </si>
@@ -701,6 +702,207 @@
   </si>
   <si>
     <t>sliding window</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/count-subarrays-with-score-less-than-k/</t>
+  </si>
+  <si>
+    <t>2302. Count Subarrays With Score Less Than K</t>
+  </si>
+  <si>
+    <t>generic two poitners</t>
+  </si>
+  <si>
+    <t>2336. Smallest Number in Infinite Set</t>
+  </si>
+  <si>
+    <t>Constraint give it away</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/all-ancestors-of-a-node-in-a-directed-acyclic-graph/</t>
+  </si>
+  <si>
+    <t>2192. All Ancestors of a Node in a Directed Acyclic Graph</t>
+  </si>
+  <si>
+    <t>Topologcial sort</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/sum-of-subarray-ranges/</t>
+  </si>
+  <si>
+    <t>2104. Sum of Subarray Ranges</t>
+  </si>
+  <si>
+    <t>monotonic stacs</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/capacity-to-ship-packages-within-d-days/</t>
+  </si>
+  <si>
+    <t>1011. Capacity To Ship Packages Within D Days</t>
+  </si>
+  <si>
+    <t>Binary Search</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/employee-free-time/</t>
+  </si>
+  <si>
+    <t>759. Employee Free Time</t>
+  </si>
+  <si>
+    <t>sometimes, they look like merge sort, but actually, you only need to sort once, and then merge together. Don’t over think</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/subarray-sums-divisible-by-k/</t>
+  </si>
+  <si>
+    <t>974. Subarray Sums Divisible by K</t>
+  </si>
+  <si>
+    <t>a = (a + mod) % mod</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-cost-tree-from-leaf-values/</t>
+  </si>
+  <si>
+    <t>1130. Minimum Cost Tree From Leaf Values</t>
+  </si>
+  <si>
+    <t>monotonic stack, consuming smallest values</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/online-stock-span/</t>
+  </si>
+  <si>
+    <t>901. Online Stock Span</t>
+  </si>
+  <si>
+    <t>monotonic stack</t>
+  </si>
+  <si>
+    <t>1249. Minimum Remove to Make Valid Parentheses</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-remove-to-make-valid-parentheses/</t>
+  </si>
+  <si>
+    <t>use stack it is easier</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/shortest-word-distance-ii/</t>
+  </si>
+  <si>
+    <t>244. Shortest Word Distance II</t>
+  </si>
+  <si>
+    <t>HashMap motherfuckers!</t>
+  </si>
+  <si>
+    <t>2045. Second Minimum Time to Reach Destination</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/second-minimum-time-to-reach-destination/</t>
+  </si>
+  <si>
+    <t>Dijkstra Algorithm</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/find-all-lonely-numbers-in-the-array/</t>
+  </si>
+  <si>
+    <t>Arrays</t>
+  </si>
+  <si>
+    <t>2150. Find All Lonely Numbers in the Array</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/number-of-ways-to-stay-in-the-same-place-after-some-steps/</t>
+  </si>
+  <si>
+    <t>1269. Number of Ways to Stay in the Same Place After Some Steps</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/bulb-switcher</t>
+  </si>
+  <si>
+    <t>Math problem</t>
+  </si>
+  <si>
+    <t>319. Bulb Switcher</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-number-of-points-with-cost/</t>
+  </si>
+  <si>
+    <t>1937. Maximum Number of Points with Cost</t>
+  </si>
+  <si>
+    <t>Kadane</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/car-fleet/</t>
+  </si>
+  <si>
+    <t>853. Car Fleet</t>
+  </si>
+  <si>
+    <t>1014. Best Sightseeing Pair</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/best-sightseeing-pair/</t>
+  </si>
+  <si>
+    <t>1626. Best Team With No Conflicts</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/best-team-with-no-conflicts/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/toss-strange-coins/</t>
+  </si>
+  <si>
+    <t>1230. Toss Strange Coins</t>
+  </si>
+  <si>
+    <t>Math</t>
+  </si>
+  <si>
+    <t>1255. Maximum Score Words Formed by Letters</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-score-words-formed-by-letters/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/reducing-dishes/</t>
+  </si>
+  <si>
+    <t>1402. Reducing Dishes</t>
+  </si>
+  <si>
+    <t>857. Minimum Cost to Hire K Workers</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-cost-to-hire-k-workers/</t>
+  </si>
+  <si>
+    <t>Heap</t>
+  </si>
+  <si>
+    <t>Logical Thinking</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-compatibility-score-sum/description/</t>
+  </si>
+  <si>
+    <t>1947. Maximum Compatibility Score Sum</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-falling-path-sum-ii/description/</t>
+  </si>
+  <si>
+    <t>1289. Minimum Falling Path Sum II</t>
   </si>
 </sst>
 </file>
@@ -802,7 +1004,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -862,12 +1064,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="41">
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1018,6 +1221,9 @@
       <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1050,23 +1256,36 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D7" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D7" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
   <autoFilter ref="A1:D7"/>
   <tableColumns count="4">
-    <tableColumn id="4" name="Date" dataDxfId="37">
+    <tableColumn id="4" name="Date" dataDxfId="38">
       <calculatedColumnFormula>D</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Name" dataDxfId="36"/>
-    <tableColumn id="2" name="Link" dataDxfId="35" dataCellStyle="Hyperlink"/>
-    <tableColumn id="3" name="Logical Thinking Process" dataDxfId="34"/>
+    <tableColumn id="1" name="Name" dataDxfId="37"/>
+    <tableColumn id="2" name="Link" dataDxfId="36" dataCellStyle="Hyperlink"/>
+    <tableColumn id="3" name="Logical Thinking Process" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A1:D41" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
-  <autoFilter ref="A1:D41"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A1:D3" totalsRowShown="0">
+  <autoFilter ref="A1:D3"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Date" dataDxfId="34"/>
+    <tableColumn id="2" name="Name"/>
+    <tableColumn id="3" name="Link" dataCellStyle="Hyperlink"/>
+    <tableColumn id="4" name="Logical Thinking"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A1:D50" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+  <autoFilter ref="A1:D50"/>
   <sortState ref="A2:D41">
     <sortCondition ref="A1:A41"/>
   </sortState>
@@ -1082,7 +1301,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:D5" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25" totalsRowBorderDxfId="24">
   <autoFilter ref="A1:D5"/>
   <tableColumns count="4">
@@ -1095,9 +1314,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table143" displayName="Table143" ref="A1:D18" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="A1:D18"/>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table143" displayName="Table143" ref="A1:D30" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="A1:D30"/>
   <tableColumns count="4">
     <tableColumn id="4" name="Date" dataDxfId="21"/>
     <tableColumn id="1" name="Name" dataDxfId="20"/>
@@ -1108,7 +1327,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table14356" displayName="Table14356" ref="A1:D6" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="A1:D6"/>
   <tableColumns count="4">
@@ -1121,9 +1340,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table1435" displayName="Table1435" ref="A1:D6" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:D6"/>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table1435" displayName="Table1435" ref="A1:D9" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:D9"/>
   <tableColumns count="4">
     <tableColumn id="4" name="Date" dataDxfId="9"/>
     <tableColumn id="1" name="Name" dataDxfId="8"/>
@@ -1134,7 +1353,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table14358" displayName="Table14358" ref="A1:D6" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A1:D6"/>
   <tableColumns count="4">
@@ -1413,7 +1632,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1536,15 +1755,74 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="23">
+        <v>44897</v>
+      </c>
+      <c r="B2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="D2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="23"/>
+      <c r="C3" s="6"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="60.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50" style="1" customWidth="1"/>
     <col min="4" max="4" width="75.6640625" style="1" bestFit="1" customWidth="1"/>
@@ -2113,6 +2391,128 @@
       </c>
       <c r="D41" s="4" t="s">
         <v>201</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A42" s="3">
+        <v>44833</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="D42" s="4"/>
+    </row>
+    <row r="43" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A43" s="3">
+        <v>44859</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="3">
+        <v>44878</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="3">
+        <v>44886</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="3">
+        <v>44888</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A47" s="3">
+        <v>44892</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="D47" s="4"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="3">
+        <v>44896</v>
+      </c>
+      <c r="B48" t="s">
+        <v>274</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A49" s="3">
+        <v>44902</v>
+      </c>
+      <c r="B49" t="s">
+        <v>280</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A50" s="3">
+        <v>44904</v>
+      </c>
+      <c r="B50" t="s">
+        <v>282</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2126,16 +2526,19 @@
     <hyperlink ref="C19" r:id="rId7"/>
     <hyperlink ref="C26" r:id="rId8"/>
     <hyperlink ref="C41" r:id="rId9"/>
+    <hyperlink ref="C34" r:id="rId10"/>
+    <hyperlink ref="C44" r:id="rId11"/>
+    <hyperlink ref="C45" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId13"/>
   <tableParts count="1">
-    <tablePart r:id="rId11"/>
+    <tablePart r:id="rId14"/>
   </tableParts>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K9"/>
   <sheetViews>
@@ -2206,17 +2609,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView topLeftCell="B19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="54.109375" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="63.44140625" style="4" bestFit="1" customWidth="1"/>
@@ -2475,18 +2878,189 @@
         <v>215</v>
       </c>
     </row>
+    <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>44785</v>
+      </c>
+      <c r="B19" t="s">
+        <v>217</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>44786</v>
+      </c>
+      <c r="B20" t="s">
+        <v>219</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>44787</v>
+      </c>
+      <c r="B21" t="s">
+        <v>225</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>44787</v>
+      </c>
+      <c r="B22" t="s">
+        <v>228</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>44789</v>
+      </c>
+      <c r="B23" t="s">
+        <v>234</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>44791</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>44791</v>
+      </c>
+      <c r="B25" t="s">
+        <v>240</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>44803</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <v>44808</v>
+      </c>
+      <c r="B27" t="s">
+        <v>246</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>44852</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
+        <v>44854</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
+        <v>44870</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C16" r:id="rId1"/>
+    <hyperlink ref="C19" r:id="rId2"/>
+    <hyperlink ref="C28" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -2598,18 +3172,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D6"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="56.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="65.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="10" width="8.88671875" style="1"/>
@@ -2701,23 +3275,68 @@
         <v>117</v>
       </c>
     </row>
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>44786</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>44814</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>44817</v>
+      </c>
+      <c r="B9" t="s">
+        <v>253</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>252</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C7" r:id="rId2"/>
+    <hyperlink ref="C8" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2757,10 +3376,19 @@
         <v>153</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="4"/>
+    <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>44789</v>
+      </c>
+      <c r="B3" t="s">
+        <v>231</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>

</xml_diff>

<commit_message>
Recent development, pracitces, learnings
</commit_message>
<xml_diff>
--- a/LCProblems.xlsx
+++ b/LCProblems.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="285">
   <si>
     <t>https://leetcode.com/problems/regions-cut-by-slashes</t>
   </si>
@@ -903,6 +903,12 @@
   </si>
   <si>
     <t>1289. Minimum Falling Path Sum II</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/count-number-of-ways-to-place-houses/description/</t>
+  </si>
+  <si>
+    <t>2320. Count Number of Ways to Place Houses</t>
   </si>
 </sst>
 </file>
@@ -1284,8 +1290,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A1:D50" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
-  <autoFilter ref="A1:D50"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A1:D51" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+  <autoFilter ref="A1:D51"/>
   <sortState ref="A2:D41">
     <sortCondition ref="A1:A41"/>
   </sortState>
@@ -1814,10 +1820,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="C43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2512,6 +2518,20 @@
         <v>281</v>
       </c>
       <c r="D50" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A51" s="3">
+        <v>44925</v>
+      </c>
+      <c r="B51" t="s">
+        <v>284</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="D51" s="4" t="s">
         <v>76</v>
       </c>
     </row>

</xml_diff>

<commit_message>
last updates from Thales Laptop
</commit_message>
<xml_diff>
--- a/LCProblems.xlsx
+++ b/LCProblems.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6228" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6228" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Union Find" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="299">
   <si>
     <t>https://leetcode.com/problems/regions-cut-by-slashes</t>
   </si>
@@ -945,6 +945,12 @@
   </si>
   <si>
     <t>Balance Binary Search Tree</t>
+  </si>
+  <si>
+    <t>945. Minimum Increment to Make Array Unique</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-increment-to-make-array-unique/description/</t>
   </si>
 </sst>
 </file>
@@ -1046,7 +1052,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1107,12 +1113,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="41">
+  <dxfs count="45">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1130,7 +1155,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1149,7 +1174,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1263,9 +1288,6 @@
       <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1298,53 +1320,53 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D7" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D7" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
   <autoFilter ref="A1:D7"/>
   <tableColumns count="4">
-    <tableColumn id="4" name="Date" dataDxfId="38">
+    <tableColumn id="4" name="Date" dataDxfId="42">
       <calculatedColumnFormula>D</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Name" dataDxfId="37"/>
-    <tableColumn id="2" name="Link" dataDxfId="36" dataCellStyle="Hyperlink"/>
-    <tableColumn id="3" name="Logical Thinking Process" dataDxfId="35"/>
+    <tableColumn id="1" name="Name" dataDxfId="41"/>
+    <tableColumn id="2" name="Link" dataDxfId="40" dataCellStyle="Hyperlink"/>
+    <tableColumn id="3" name="Logical Thinking Process" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A1:D3" totalsRowShown="0">
-  <autoFilter ref="A1:D3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A1:D4" totalsRowShown="0" dataDxfId="0">
+  <autoFilter ref="A1:D4"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Date" dataDxfId="34"/>
-    <tableColumn id="2" name="Name"/>
-    <tableColumn id="3" name="Link" dataCellStyle="Hyperlink"/>
-    <tableColumn id="4" name="Logical Thinking"/>
+    <tableColumn id="1" name="Date" dataDxfId="4"/>
+    <tableColumn id="2" name="Name" dataDxfId="3"/>
+    <tableColumn id="3" name="Link" dataDxfId="2" dataCellStyle="Hyperlink"/>
+    <tableColumn id="4" name="Logical Thinking" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A1:D53" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A1:D53" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
   <autoFilter ref="A1:D53"/>
   <sortState ref="A2:D41">
     <sortCondition ref="A1:A41"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="4" name="Date" dataDxfId="31">
+    <tableColumn id="4" name="Date" dataDxfId="36">
       <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Name" dataDxfId="30"/>
-    <tableColumn id="2" name="Link" dataDxfId="29" dataCellStyle="Hyperlink"/>
-    <tableColumn id="3" name="Logical Thinking Process" dataDxfId="28"/>
+    <tableColumn id="1" name="Name" dataDxfId="35"/>
+    <tableColumn id="2" name="Link" dataDxfId="34" dataCellStyle="Hyperlink"/>
+    <tableColumn id="3" name="Logical Thinking Process" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:D5" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25" totalsRowBorderDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:D5" totalsRowShown="0" headerRowDxfId="32" headerRowBorderDxfId="31" tableBorderDxfId="30" totalsRowBorderDxfId="29">
   <autoFilter ref="A1:D5"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Date"/>
@@ -1357,52 +1379,52 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table143" displayName="Table143" ref="A1:D31" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table143" displayName="Table143" ref="A1:D31" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="A1:D31"/>
   <tableColumns count="4">
-    <tableColumn id="4" name="Date" dataDxfId="21"/>
-    <tableColumn id="1" name="Name" dataDxfId="20"/>
-    <tableColumn id="2" name="Link" dataDxfId="19" dataCellStyle="Hyperlink"/>
-    <tableColumn id="3" name="Logical Thinking Process" dataDxfId="18"/>
+    <tableColumn id="4" name="Date" dataDxfId="26"/>
+    <tableColumn id="1" name="Name" dataDxfId="25"/>
+    <tableColumn id="2" name="Link" dataDxfId="24" dataCellStyle="Hyperlink"/>
+    <tableColumn id="3" name="Logical Thinking Process" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table14356" displayName="Table14356" ref="A1:D6" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table14356" displayName="Table14356" ref="A1:D6" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
   <autoFilter ref="A1:D6"/>
   <tableColumns count="4">
-    <tableColumn id="4" name="Date" dataDxfId="15"/>
-    <tableColumn id="1" name="Name" dataDxfId="14"/>
-    <tableColumn id="2" name="Link" dataDxfId="13" dataCellStyle="Hyperlink"/>
-    <tableColumn id="3" name="Logical Thinking Process" dataDxfId="12"/>
+    <tableColumn id="4" name="Date" dataDxfId="20"/>
+    <tableColumn id="1" name="Name" dataDxfId="19"/>
+    <tableColumn id="2" name="Link" dataDxfId="18" dataCellStyle="Hyperlink"/>
+    <tableColumn id="3" name="Logical Thinking Process" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table1435" displayName="Table1435" ref="A1:D11" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table1435" displayName="Table1435" ref="A1:D11" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="A1:D11"/>
   <tableColumns count="4">
-    <tableColumn id="4" name="Date" dataDxfId="3"/>
-    <tableColumn id="1" name="Name" dataDxfId="2"/>
-    <tableColumn id="2" name="Link" dataDxfId="1" dataCellStyle="Hyperlink"/>
-    <tableColumn id="3" name="Logical Thinking Process" dataDxfId="0"/>
+    <tableColumn id="4" name="Date" dataDxfId="14"/>
+    <tableColumn id="1" name="Name" dataDxfId="13"/>
+    <tableColumn id="2" name="Link" dataDxfId="12" dataCellStyle="Hyperlink"/>
+    <tableColumn id="3" name="Logical Thinking Process" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table14358" displayName="Table14358" ref="A1:D6" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table14358" displayName="Table14358" ref="A1:D6" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A1:D6"/>
   <tableColumns count="4">
-    <tableColumn id="4" name="Date" dataDxfId="9"/>
-    <tableColumn id="1" name="Name" dataDxfId="8"/>
-    <tableColumn id="2" name="Link" dataDxfId="7" dataCellStyle="Hyperlink"/>
-    <tableColumn id="3" name="Logical Thinking Process" dataDxfId="6"/>
+    <tableColumn id="4" name="Date" dataDxfId="8"/>
+    <tableColumn id="1" name="Name" dataDxfId="7"/>
+    <tableColumn id="2" name="Link" dataDxfId="6" dataCellStyle="Hyperlink"/>
+    <tableColumn id="3" name="Logical Thinking Process" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1797,17 +1819,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="71.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="74.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1826,41 +1848,56 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="23">
+      <c r="A2" s="24">
         <v>44897</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="20" t="s">
         <v>276</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="23">
+      <c r="A3" s="24">
         <v>45021</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="20" t="s">
         <v>289</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>290</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="24">
+        <v>45034</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>298</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3277,8 +3314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>